<commit_message>
update excel & package name fix
</commit_message>
<xml_diff>
--- a/Project2/TaskDistribution.xlsx
+++ b/Project2/TaskDistribution.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HKIE_BOOTCAMP\HKIE-Project\Project2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12225" windowHeight="6915"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12228" windowHeight="6912"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:F21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Common</t>
   </si>
@@ -92,13 +96,19 @@
   </si>
   <si>
     <t>Candy</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Sunny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +145,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -181,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,9 +231,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,6 +283,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,22 +476,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -451,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -465,15 +519,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -481,7 +538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -495,7 +552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -503,7 +560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -517,7 +574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -528,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -542,7 +599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -553,12 +610,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -567,24 +627,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
addDish use session merchant id
</commit_message>
<xml_diff>
--- a/Project2/TaskDistribution.xlsx
+++ b/Project2/TaskDistribution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Common</t>
   </si>
@@ -469,7 +469,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,6 +609,9 @@
       </c>
       <c r="E9" t="s">
         <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6">

</xml_diff>